<commit_message>
Paths relative to Excel file. Update triangular so high != low
</commit_message>
<xml_diff>
--- a/tests/fmudesign/data/config/design_input_background_no_seed.xlsx
+++ b/tests/fmudesign/data/config/design_input_background_no_seed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\fmu\users\tral\fmu-utils\github\fmu-tools\tests\data\sensitivities\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appl\github\semeio\tests\fmudesign\data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED9ACEC-62C1-4A0A-98D9-B84C33A88F74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5A29AF-BDF7-44D2-BF37-F9F3827A7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2055" windowWidth="27240" windowHeight="13815" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -467,9 +467,6 @@
     <t>PARAM13</t>
   </si>
   <si>
-    <t>tests/data/sensitivities/config/doe1.xlsx</t>
-  </si>
-  <si>
     <t>PARAM14</t>
   </si>
   <si>
@@ -519,6 +516,9 @@
   </si>
   <si>
     <t>rms_seeds</t>
+  </si>
+  <si>
+    <t>doe1.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1364,10 +1364,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1402,13 +1402,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1429,13 +1429,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1456,14 +1456,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1486,13 +1486,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1517,9 +1517,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1532,7 +1532,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1545,8 +1545,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1567,20 +1567,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1593,17 +1593,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1621,20 +1621,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1646,16 +1646,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1665,43 +1665,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1732,9 +1731,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1748,14 +1744,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2403,9 +2399,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2443,7 +2439,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2549,7 +2545,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2691,7 +2687,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2731,7 +2727,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -2757,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,7 +3180,7 @@
       <c r="D14" s="147" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="157"/>
+      <c r="E14" s="148"/>
       <c r="F14" s="145"/>
       <c r="G14" s="145"/>
       <c r="H14" s="149"/>
@@ -3214,7 +3210,7 @@
       <c r="D15" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="157"/>
+      <c r="E15" s="148"/>
       <c r="F15" s="145"/>
       <c r="G15" s="145"/>
       <c r="H15" s="149"/>
@@ -3224,11 +3220,11 @@
       <c r="J15" s="151">
         <v>1</v>
       </c>
-      <c r="K15" s="152">
-        <v>1</v>
+      <c r="K15" s="190">
+        <v>1.5</v>
       </c>
       <c r="L15" s="153">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="154"/>
       <c r="N15" s="154"/>
@@ -3238,28 +3234,28 @@
       <c r="P15" s="156"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="158"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="160"/>
-      <c r="D16" s="161" t="s">
+      <c r="A16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="160" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="162"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="164" t="s">
+      <c r="E16" s="161"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="162"/>
+      <c r="I16" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="165">
+      <c r="J16" s="164">
         <v>1</v>
       </c>
-      <c r="K16" s="166">
+      <c r="K16" s="165">
         <v>10</v>
       </c>
-      <c r="L16" s="167"/>
-      <c r="M16" s="168"/>
-      <c r="N16" s="168"/>
+      <c r="L16" s="166"/>
+      <c r="M16" s="167"/>
+      <c r="N16" s="167"/>
       <c r="O16" s="155" t="s">
         <v>54</v>
       </c>
@@ -3278,19 +3274,19 @@
       <c r="D17" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="169"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="171"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="170"/>
       <c r="I17" s="114"/>
       <c r="J17" s="115"/>
       <c r="K17" s="116"/>
       <c r="L17" s="117"/>
       <c r="M17" s="118"/>
       <c r="N17" s="118"/>
-      <c r="O17" s="172"/>
+      <c r="O17" s="171"/>
       <c r="P17" s="119" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3298,19 +3294,19 @@
       <c r="B18" s="121"/>
       <c r="C18" s="122"/>
       <c r="D18" s="123" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="173"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="175"/>
+        <v>61</v>
+      </c>
+      <c r="E18" s="172"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="173"/>
+      <c r="H18" s="174"/>
       <c r="I18" s="126"/>
       <c r="J18" s="127"/>
       <c r="K18" s="128"/>
       <c r="L18" s="129"/>
       <c r="M18" s="130"/>
       <c r="N18" s="130"/>
-      <c r="O18" s="176"/>
+      <c r="O18" s="175"/>
       <c r="P18" s="131"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3318,19 +3314,19 @@
       <c r="B19" s="121"/>
       <c r="C19" s="122"/>
       <c r="D19" s="123" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="173"/>
-      <c r="F19" s="174"/>
-      <c r="G19" s="174"/>
-      <c r="H19" s="175"/>
+        <v>62</v>
+      </c>
+      <c r="E19" s="172"/>
+      <c r="F19" s="173"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="174"/>
       <c r="I19" s="126"/>
       <c r="J19" s="127"/>
       <c r="K19" s="128"/>
       <c r="L19" s="129"/>
       <c r="M19" s="130"/>
       <c r="N19" s="130"/>
-      <c r="O19" s="176"/>
+      <c r="O19" s="175"/>
       <c r="P19" s="131"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3338,19 +3334,19 @@
       <c r="B20" s="133"/>
       <c r="C20" s="134"/>
       <c r="D20" s="135" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="177"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="178"/>
-      <c r="H20" s="179"/>
+        <v>63</v>
+      </c>
+      <c r="E20" s="176"/>
+      <c r="F20" s="177"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="178"/>
       <c r="I20" s="138"/>
       <c r="J20" s="139"/>
       <c r="K20" s="140"/>
       <c r="L20" s="141"/>
       <c r="M20" s="142"/>
       <c r="N20" s="142"/>
-      <c r="O20" s="180"/>
+      <c r="O20" s="179"/>
       <c r="P20" s="143"/>
     </row>
   </sheetData>
@@ -3381,12 +3377,12 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -3394,15 +3390,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -3421,7 +3417,7 @@
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3453,7 +3449,7 @@
         <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3482,7 +3478,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -3530,7 +3526,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
@@ -3538,7 +3534,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
@@ -3546,7 +3542,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
@@ -3554,7 +3550,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
@@ -3562,7 +3558,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
@@ -3570,7 +3566,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -3581,7 +3577,7 @@
         <v>47</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -3623,55 +3619,55 @@
       <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="181">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="181" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="181">
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="181">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="181" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="181">
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="181"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="181">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5" s="181">
+      <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="181">
+      <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="181">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3698,97 +3694,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="182" t="s">
+      <c r="A1" s="180" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="183" t="s">
+      <c r="B1" s="181" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="184" t="s">
+      <c r="C1" s="182" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="185" t="s">
+      <c r="D1" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="185" t="s">
+      <c r="E1" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="185" t="s">
+      <c r="F1" s="183" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="185" t="s">
+      <c r="G1" s="183" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="186" t="s">
+      <c r="H1" s="184" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="185" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="186" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="187">
+        <v>0</v>
+      </c>
+      <c r="D2" s="187">
+        <v>1</v>
+      </c>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187">
+        <v>2</v>
+      </c>
+      <c r="H2" s="155" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="188" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="188" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="189">
+      <c r="B3" s="189" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="189">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="155" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="190" t="s">
+      <c r="H3" s="155" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="188" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="191" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="192">
-        <v>0</v>
-      </c>
-      <c r="D3" s="192">
+      <c r="B4" s="189" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192">
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="155" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="190" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="191" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="192">
-        <v>1</v>
-      </c>
-      <c r="D4" s="192">
-        <v>3</v>
-      </c>
-      <c r="E4" s="192">
-        <v>5</v>
-      </c>
-      <c r="F4" s="192"/>
-      <c r="G4" s="192">
-        <v>2</v>
-      </c>
       <c r="H4" s="155" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3818,48 +3814,48 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="181">
+        <v>72</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="181" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="181">
+        <v>73</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="181"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="181">
-        <v>0</v>
-      </c>
-      <c r="C4" s="181" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="181">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>